<commit_message>
Added a Public PNR Status Feature
</commit_message>
<xml_diff>
--- a/agile_documents/Agile Document - Aditya Kumar.xlsx
+++ b/agile_documents/Agile Document - Aditya Kumar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -221,9 +221,6 @@
     <t>Day 12</t>
   </si>
   <si>
-    <t>Day 13</t>
-  </si>
-  <si>
     <t>T1.1</t>
   </si>
   <si>
@@ -348,6 +345,9 @@
   </si>
   <si>
     <t>Data Viz</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
   <si>
     <t>SL</t>
@@ -529,7 +529,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -543,6 +543,12 @@
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1005,152 +1011,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1164,6 +1170,10 @@
     <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,21 +1226,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="59">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-        <charset val="134"/>
-        <family val="0"/>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-      </font>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <font>
         <name val="Arial"/>
@@ -1981,29 +1977,29 @@
     </dxf>
   </dxfs>
   <tableStyles count="4">
-    <tableStyle name="Product Backlog-style" pivot="0" count="4" xr9:uid="{3AAAB6B5-48E6-4222-AEFB-C1D91AE4734E}">
-      <tableStyleElement type="wholeTable" dxfId="46"/>
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
-      <tableStyleElement type="secondRowStripe" dxfId="43"/>
+    <tableStyle name="Product Backlog-style" pivot="0" count="4" xr9:uid="{A44AA518-42BB-4DC7-8E98-27480B1E3508}">
+      <tableStyleElement type="wholeTable" dxfId="45"/>
+      <tableStyleElement type="headerRow" dxfId="44"/>
+      <tableStyleElement type="firstRowStripe" dxfId="43"/>
+      <tableStyleElement type="secondRowStripe" dxfId="42"/>
     </tableStyle>
-    <tableStyle name="Sprint Backlog-style" pivot="0" count="4" xr9:uid="{D7074E4E-E4DE-4A27-9D72-54409DFF041B}">
-      <tableStyleElement type="wholeTable" dxfId="50"/>
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="firstRowStripe" dxfId="48"/>
-      <tableStyleElement type="secondRowStripe" dxfId="47"/>
+    <tableStyle name="Sprint Backlog-style" pivot="0" count="4" xr9:uid="{C087593B-4791-407F-93AD-EA305C216948}">
+      <tableStyleElement type="wholeTable" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
+      <tableStyleElement type="firstRowStripe" dxfId="47"/>
+      <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="Retrospection-style" pivot="0" count="4" xr9:uid="{C4A8C721-930A-469D-9853-AFAF31CABFDC}">
-      <tableStyleElement type="wholeTable" dxfId="54"/>
-      <tableStyleElement type="headerRow" dxfId="53"/>
-      <tableStyleElement type="firstRowStripe" dxfId="52"/>
-      <tableStyleElement type="secondRowStripe" dxfId="51"/>
+    <tableStyle name="Retrospection-style" pivot="0" count="4" xr9:uid="{28BDD1B0-1D11-4EF8-B4EA-54EEBEBBBBA5}">
+      <tableStyleElement type="wholeTable" dxfId="53"/>
+      <tableStyleElement type="headerRow" dxfId="52"/>
+      <tableStyleElement type="firstRowStripe" dxfId="51"/>
+      <tableStyleElement type="secondRowStripe" dxfId="50"/>
     </tableStyle>
-    <tableStyle name="Stand up Meeting-style" pivot="0" count="4" xr9:uid="{F6A8561F-9373-4ED9-BF09-C00A3D1518F3}">
-      <tableStyleElement type="wholeTable" dxfId="58"/>
-      <tableStyleElement type="headerRow" dxfId="57"/>
-      <tableStyleElement type="firstRowStripe" dxfId="56"/>
-      <tableStyleElement type="secondRowStripe" dxfId="55"/>
+    <tableStyle name="Stand up Meeting-style" pivot="0" count="4" xr9:uid="{5B9F1FF7-461E-4D7C-8308-652708B82841}">
+      <tableStyleElement type="wholeTable" dxfId="57"/>
+      <tableStyleElement type="headerRow" dxfId="56"/>
+      <tableStyleElement type="firstRowStripe" dxfId="55"/>
+      <tableStyleElement type="secondRowStripe" dxfId="54"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2031,8 +2027,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Sprint_Backlog" displayName="Sprint_Backlog" ref="A1:V14">
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Sprint_Backlog" displayName="Sprint_Backlog" ref="A1:U15">
+  <tableColumns count="21">
     <tableColumn id="1" name="US ID" dataDxfId="8"/>
     <tableColumn id="2" name="Task ID" dataDxfId="9"/>
     <tableColumn id="3" name="Task Description" dataDxfId="10"/>
@@ -2054,7 +2050,6 @@
     <tableColumn id="19" name="Day 10" dataDxfId="26"/>
     <tableColumn id="20" name="Day 11" dataDxfId="27"/>
     <tableColumn id="21" name="Day 12" dataDxfId="28"/>
-    <tableColumn id="22" name="Day 13" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="Sprint Backlog-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2063,15 +2058,15 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Retrospection" displayName="Retrospection" ref="A1:I7">
   <tableColumns count="9">
-    <tableColumn id="1" name="SL" dataDxfId="30"/>
-    <tableColumn id="2" name="Sprint" dataDxfId="31"/>
-    <tableColumn id="3" name="Start Date" dataDxfId="32"/>
-    <tableColumn id="4" name="End Date" dataDxfId="33"/>
-    <tableColumn id="5" name="Team Member Name" dataDxfId="34"/>
-    <tableColumn id="6" name="Start Doing" dataDxfId="35"/>
-    <tableColumn id="7" name="Stop Doing" dataDxfId="36"/>
-    <tableColumn id="8" name="Continue Doing" dataDxfId="37"/>
-    <tableColumn id="9" name="Action Taken" dataDxfId="38"/>
+    <tableColumn id="1" name="SL" dataDxfId="29"/>
+    <tableColumn id="2" name="Sprint" dataDxfId="30"/>
+    <tableColumn id="3" name="Start Date" dataDxfId="31"/>
+    <tableColumn id="4" name="End Date" dataDxfId="32"/>
+    <tableColumn id="5" name="Team Member Name" dataDxfId="33"/>
+    <tableColumn id="6" name="Start Doing" dataDxfId="34"/>
+    <tableColumn id="7" name="Stop Doing" dataDxfId="35"/>
+    <tableColumn id="8" name="Continue Doing" dataDxfId="36"/>
+    <tableColumn id="9" name="Action Taken" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="Retrospection-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2080,10 +2075,10 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Stand_up_Meeting" displayName="Stand_up_Meeting" ref="A1:D11">
   <tableColumns count="4">
-    <tableColumn id="1" name="Sprint" dataDxfId="39"/>
-    <tableColumn id="2" name="Day" dataDxfId="40"/>
-    <tableColumn id="3" name="Impediments" dataDxfId="41"/>
-    <tableColumn id="4" name="Action Taken" dataDxfId="42"/>
+    <tableColumn id="1" name="Sprint" dataDxfId="38"/>
+    <tableColumn id="2" name="Day" dataDxfId="39"/>
+    <tableColumn id="3" name="Impediments" dataDxfId="40"/>
+    <tableColumn id="4" name="Action Taken" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="Stand up Meeting-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2291,7 +2286,7 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
@@ -2299,14 +2294,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="9.5" customWidth="1"/>
-    <col min="4" max="4" width="97.6296296296296" customWidth="1"/>
-    <col min="5" max="5" width="15.6296296296296" customWidth="1"/>
-    <col min="6" max="6" width="14.6296296296296" customWidth="1"/>
-    <col min="7" max="7" width="13.3796296296296" customWidth="1"/>
-    <col min="8" max="8" width="10.3796296296296" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="12.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="7.11111111111111" customWidth="1"/>
+    <col min="4" max="4" width="118.222222222222" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="15.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="14.4444444444444" customWidth="1"/>
+    <col min="8" max="8" width="10.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1" spans="1:8">
@@ -2614,17 +2609,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.11111111111111" customWidth="1"/>
+    <col min="1" max="1" width="7.22222222222222" customWidth="1"/>
     <col min="2" max="2" width="7.88888888888889" customWidth="1"/>
     <col min="3" max="3" width="47.5555555555556" customWidth="1"/>
     <col min="4" max="5" width="11.1111111111111" customWidth="1"/>
@@ -2633,10 +2628,10 @@
     <col min="8" max="8" width="6.66666666666667" customWidth="1"/>
     <col min="9" max="9" width="9.44444444444444" customWidth="1"/>
     <col min="10" max="18" width="6.55555555555556" customWidth="1"/>
-    <col min="19" max="19" width="7.55555555555556" customWidth="1"/>
+    <col min="19" max="21" width="7.55555555555556" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.5" customHeight="1" spans="1:22">
+    <row r="1" ht="22.5" customHeight="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2700,19 +2695,16 @@
       <c r="U1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" ht="22.5" customHeight="1" spans="1:11">
+    </row>
+    <row r="2" ht="22.5" customHeight="1" spans="1:21">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D2" s="4">
         <v>45979</v>
@@ -2721,33 +2713,43 @@
         <v>45980</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" s="2">
-        <v>8</v>
-      </c>
-      <c r="J2" s="2">
-        <v>4</v>
-      </c>
-      <c r="K2" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="22.5" customHeight="1" spans="1:13">
+      <c r="I2" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+    </row>
+    <row r="3" ht="22.5" customHeight="1" spans="1:21">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D3" s="4">
         <v>45981</v>
@@ -2756,33 +2758,43 @@
         <v>45982</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="2">
-        <v>6</v>
-      </c>
-      <c r="L3" s="2">
-        <v>3</v>
-      </c>
-      <c r="M3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" ht="22.5" customHeight="1" spans="1:16">
+        <v>67</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" ht="22.5" customHeight="1" spans="1:21">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D4" s="4">
         <v>45985</v>
@@ -2791,36 +2803,45 @@
         <v>45987</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" s="2">
-        <v>10</v>
-      </c>
-      <c r="N4" s="2">
-        <v>4</v>
-      </c>
-      <c r="O4" s="2">
-        <v>4</v>
-      </c>
-      <c r="P4" s="2">
+        <v>67</v>
+      </c>
+      <c r="I4" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" ht="22.5" customHeight="1" spans="1:19">
+      <c r="O4" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="P4" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" ht="22.5" customHeight="1" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="4">
         <v>45988</v>
@@ -2829,36 +2850,45 @@
         <v>45991</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="2">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>4</v>
-      </c>
-      <c r="R5" s="2">
-        <v>4</v>
-      </c>
-      <c r="S5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" ht="22.5" customHeight="1" spans="1:12">
+        <v>67</v>
+      </c>
+      <c r="I5" s="5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="5">
+        <v>2</v>
+      </c>
+      <c r="R5" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" ht="22.5" customHeight="1" spans="1:21">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D6" s="4">
         <v>45992</v>
@@ -2867,36 +2897,43 @@
         <v>45994</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="2">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2">
-        <v>4</v>
-      </c>
-      <c r="K6" s="2">
-        <v>4</v>
-      </c>
-      <c r="L6" s="2">
+        <v>67</v>
+      </c>
+      <c r="I6" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="J6" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="K6" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" ht="22.5" customHeight="1" spans="1:16">
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" ht="22.5" customHeight="1" spans="1:21">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D7" s="4">
         <v>45995</v>
@@ -2905,39 +2942,45 @@
         <v>45998</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="2">
-        <v>12</v>
-      </c>
-      <c r="M7" s="2">
-        <v>4</v>
-      </c>
-      <c r="N7" s="2">
-        <v>4</v>
-      </c>
-      <c r="O7" s="2">
+        <v>67</v>
+      </c>
+      <c r="I7" s="5">
+        <v>5</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="5">
         <v>2</v>
       </c>
-      <c r="P7" s="2">
+      <c r="N7" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" ht="22.5" customHeight="1" spans="1:19">
+      <c r="O7" s="5">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" ht="22.5" customHeight="1" spans="1:21">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D8" s="4">
         <v>45999</v>
@@ -2949,33 +2992,42 @@
         <v>29</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I8" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>3</v>
-      </c>
-      <c r="R8" s="2">
-        <v>3</v>
-      </c>
-      <c r="S8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" ht="22.5" customHeight="1" spans="1:12">
+        <v>67</v>
+      </c>
+      <c r="I8" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="5">
+        <v>2</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="T8" s="5">
+        <v>1</v>
+      </c>
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" ht="22.5" customHeight="1" spans="1:21">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="D9" s="4">
         <v>46006</v>
@@ -2984,36 +3036,45 @@
         <v>46008</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" s="2">
-        <v>8</v>
-      </c>
-      <c r="J9" s="2">
-        <v>4</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2</v>
-      </c>
-      <c r="L9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" ht="22.5" customHeight="1" spans="1:16">
+        <v>67</v>
+      </c>
+      <c r="I9" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1</v>
+      </c>
+      <c r="L9" s="5">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" ht="22.5" customHeight="1" spans="1:21">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D10" s="4">
         <v>46009</v>
@@ -3022,39 +3083,47 @@
         <v>46013</v>
       </c>
       <c r="F10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I10" s="2">
-        <v>12</v>
-      </c>
-      <c r="M10" s="2">
-        <v>4</v>
-      </c>
-      <c r="N10" s="2">
-        <v>4</v>
-      </c>
-      <c r="O10" s="2">
-        <v>2</v>
-      </c>
-      <c r="P10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" ht="22.5" customHeight="1" spans="1:19">
+        <v>67</v>
+      </c>
+      <c r="I10" s="5">
+        <v>5</v>
+      </c>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="O10" s="5">
+        <v>1</v>
+      </c>
+      <c r="P10" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" ht="22.5" customHeight="1" spans="1:21">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D11" s="4">
         <v>46014</v>
@@ -3063,36 +3132,45 @@
         <v>46017</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I11" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>3</v>
-      </c>
-      <c r="R11" s="2">
-        <v>3</v>
-      </c>
-      <c r="S11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" ht="22.5" customHeight="1" spans="1:12">
+        <v>67</v>
+      </c>
+      <c r="I11" s="5">
+        <v>4</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="5">
+        <v>1</v>
+      </c>
+      <c r="T11" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="U11" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="12" ht="22.5" customHeight="1" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="D12" s="4">
         <v>46020</v>
@@ -3101,36 +3179,45 @@
         <v>46022</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="2">
-        <v>10</v>
-      </c>
-      <c r="J12" s="2">
-        <v>4</v>
-      </c>
-      <c r="K12" s="2">
-        <v>4</v>
-      </c>
-      <c r="L12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" ht="22.5" customHeight="1" spans="1:14">
+        <v>67</v>
+      </c>
+      <c r="I12" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="L12" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" ht="22.5" customHeight="1" spans="1:21">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D13" s="4">
         <v>46023</v>
@@ -3139,33 +3226,43 @@
         <v>46024</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="2">
-        <v>6</v>
-      </c>
-      <c r="M13" s="2">
-        <v>3</v>
-      </c>
-      <c r="N13" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" ht="22.5" customHeight="1" spans="1:19">
+        <v>67</v>
+      </c>
+      <c r="I13" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="5">
+        <v>1</v>
+      </c>
+      <c r="O13" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" ht="22.5" customHeight="1" spans="1:21">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D14" s="4">
         <v>46025</v>
@@ -3174,39 +3271,85 @@
         <v>46028</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="5">
+        <v>5</v>
+      </c>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="5">
+        <v>2</v>
+      </c>
+      <c r="T14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="U14" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" ht="22.5" customHeight="1" spans="1:21">
+      <c r="A15" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I14" s="2">
-        <v>12</v>
-      </c>
-      <c r="O14" s="2">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="I15" s="5">
+        <v>54</v>
+      </c>
+      <c r="J15" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="K15" s="5">
+        <v>6</v>
+      </c>
+      <c r="L15" s="5">
+        <v>4</v>
+      </c>
+      <c r="M15" s="5">
+        <v>4.5</v>
+      </c>
+      <c r="N15" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="O15" s="5">
+        <v>5</v>
+      </c>
+      <c r="P15" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>2</v>
+      </c>
+      <c r="R15" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="S15" s="5">
+        <v>6</v>
+      </c>
+      <c r="T15" s="5">
+        <v>4</v>
+      </c>
+      <c r="U15" s="5">
         <v>3</v>
       </c>
-      <c r="P14" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>2</v>
-      </c>
-      <c r="R14" s="2">
-        <v>2</v>
-      </c>
-      <c r="S14" s="2">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" sqref="I2:I14">
-      <formula1>AND(ISNUMBER(I2),(NOT(OR(NOT(ISERROR(DATEVALUE(I2))),AND(ISNUMBER(I2),LEFT(CELL("format",I2))="D")))))</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" sqref="D2:E14">
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" sqref="D2:E15">
       <formula1>OR(NOT(ISERROR(DATEVALUE(D2))),AND(ISNUMBER(D2),LEFT(CELL("format",D2))="D"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3225,7 +3368,7 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
@@ -3233,15 +3376,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6"/>
   <cols>
-    <col min="1" max="1" width="6.37962962962963" customWidth="1"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="16.1296296296296" customWidth="1"/>
-    <col min="4" max="4" width="15.3796296296296" customWidth="1"/>
-    <col min="5" max="5" width="21.1296296296296" customWidth="1"/>
-    <col min="6" max="6" width="34.5" customWidth="1"/>
-    <col min="7" max="7" width="32.1296296296296" customWidth="1"/>
-    <col min="8" max="8" width="33.25" customWidth="1"/>
-    <col min="9" max="9" width="37.6296296296296" customWidth="1"/>
+    <col min="1" max="1" width="3.88888888888889" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="4" width="11.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="19.5555555555556" customWidth="1"/>
+    <col min="6" max="6" width="40.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="36.8888888888889" customWidth="1"/>
+    <col min="8" max="8" width="39.1111111111111" customWidth="1"/>
+    <col min="9" max="9" width="60" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1" spans="1:9">
@@ -3476,10 +3618,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="9.87962962962963" customWidth="1"/>
-    <col min="2" max="2" width="8.25" customWidth="1"/>
-    <col min="3" max="3" width="71.25" customWidth="1"/>
-    <col min="4" max="4" width="73.1296296296296" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="6.55555555555556" customWidth="1"/>
+    <col min="3" max="3" width="86.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="88.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1" spans="1:4">

</xml_diff>